<commit_message>
Add uncertaintys and corrected G
</commit_message>
<xml_diff>
--- a/CavendishExperiment.xlsx
+++ b/CavendishExperiment.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JARAINES\Documents\Daniel Litt\CavendishExperiment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{645A9D29-0C6D-45B5-B6CB-77356401A12E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8428DF60-300A-4071-9E60-21BBA12DDD8C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{1D886BEF-429E-4660-9EA4-F3E5EA03BF59}"/>
   </bookViews>
@@ -32,8 +32,80 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={5D234F63-1455-42D4-81D9-19C4EF3D4456}</author>
+    <author>tc={DBB36E26-8B85-4D33-9107-B252D723E3C8}</author>
+    <author>tc={7E5DF10E-9598-4C7A-AC3E-B50A47336E65}</author>
+    <author>tc={F95CAA28-D0F2-451C-80BA-B448744334CE}</author>
+    <author>tc={6B1F4904-C3C9-4912-A741-561A88464FCA}</author>
+    <author>tc={A7C83F0A-E0DF-4064-83F0-843BD08DF3F2}</author>
+    <author>tc={27911C3A-1FDB-49D8-8DE3-EDBAEDC01BFB}</author>
+  </authors>
+  <commentList>
+    <comment ref="A79" authorId="0" shapeId="0" xr:uid="{5D234F63-1455-42D4-81D9-19C4EF3D4456}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Radius of the small mass</t>
+      </text>
+    </comment>
+    <comment ref="A80" authorId="1" shapeId="0" xr:uid="{DBB36E26-8B85-4D33-9107-B252D723E3C8}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    The length of the lever arm</t>
+      </text>
+    </comment>
+    <comment ref="A81" authorId="2" shapeId="0" xr:uid="{7E5DF10E-9598-4C7A-AC3E-B50A47336E65}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    the distance from center of small mass to center of large mass</t>
+      </text>
+    </comment>
+    <comment ref="A82" authorId="3" shapeId="0" xr:uid="{F95CAA28-D0F2-451C-80BA-B448744334CE}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Mass of the large mass</t>
+      </text>
+    </comment>
+    <comment ref="A83" authorId="4" shapeId="0" xr:uid="{6B1F4904-C3C9-4912-A741-561A88464FCA}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Distance from meter stick to mirror</t>
+      </text>
+    </comment>
+    <comment ref="A84" authorId="5" shapeId="0" xr:uid="{A7C83F0A-E0DF-4064-83F0-843BD08DF3F2}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    distance of the laser oscillation</t>
+      </text>
+    </comment>
+    <comment ref="A85" authorId="6" shapeId="0" xr:uid="{27911C3A-1FDB-49D8-8DE3-EDBAEDC01BFB}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Period of oscillation</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="34">
   <si>
     <t>Measurements of S</t>
   </si>
@@ -107,9 +179,6 @@
     <t>Uncertainty</t>
   </si>
   <si>
-    <t>G =</t>
-  </si>
-  <si>
     <t>r (m)</t>
   </si>
   <si>
@@ -120,6 +189,37 @@
   </si>
   <si>
     <t>ΔS (m)</t>
+  </si>
+  <si>
+    <t>Calculated G =</t>
+  </si>
+  <si>
+    <t>Actual G =</t>
+  </si>
+  <si>
+    <t>Percent differrence</t>
+  </si>
+  <si>
+    <t>Correctecd value of G</t>
+  </si>
+  <si>
+    <t>β</t>
+  </si>
+  <si>
+    <r>
+      <t>G</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -130,7 +230,7 @@
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -149,6 +249,33 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Dante"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <vertAlign val="subscript"/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -200,11 +327,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -217,10 +345,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Output" xfId="1" builtinId="21"/>
+    <cellStyle name="Percent" xfId="2" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -615,7 +747,7 @@
                 <c:pt idx="29">
                   <c:v>62.2</c:v>
                 </c:pt>
-                <c:pt idx="30">
+                <c:pt idx="30" formatCode="0.0">
                   <c:v>63</c:v>
                 </c:pt>
                 <c:pt idx="31">
@@ -645,7 +777,7 @@
                 <c:pt idx="39">
                   <c:v>64.5</c:v>
                 </c:pt>
-                <c:pt idx="40">
+                <c:pt idx="40" formatCode="0.0">
                   <c:v>64</c:v>
                 </c:pt>
                 <c:pt idx="41">
@@ -669,7 +801,7 @@
                 <c:pt idx="47">
                   <c:v>57.3</c:v>
                 </c:pt>
-                <c:pt idx="48">
+                <c:pt idx="48" formatCode="0.0">
                   <c:v>56</c:v>
                 </c:pt>
                 <c:pt idx="49">
@@ -1562,15 +1694,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>754380</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>118110</xdr:rowOff>
+      <xdr:colOff>586740</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>11430</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
-      <xdr:colOff>342900</xdr:colOff>
+      <xdr:colOff>175260</xdr:colOff>
       <xdr:row>44</xdr:row>
-      <xdr:rowOff>45720</xdr:rowOff>
+      <xdr:rowOff>121920</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1596,6 +1728,12 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <person displayName="Litt, Daniel Ethan" id="{75DA31A4-1CF0-4DC1-93FC-9A3DBED522DD}" userId="Litt, Daniel Ethan" providerId="None"/>
+</personList>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1893,17 +2031,43 @@
 </a:theme>
 </file>
 
+<file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="A79" dT="2020-09-25T01:23:30.04" personId="{75DA31A4-1CF0-4DC1-93FC-9A3DBED522DD}" id="{5D234F63-1455-42D4-81D9-19C4EF3D4456}">
+    <text>Radius of the small mass</text>
+  </threadedComment>
+  <threadedComment ref="A80" dT="2020-09-25T01:22:17.54" personId="{75DA31A4-1CF0-4DC1-93FC-9A3DBED522DD}" id="{DBB36E26-8B85-4D33-9107-B252D723E3C8}">
+    <text>The length of the lever arm</text>
+  </threadedComment>
+  <threadedComment ref="A81" dT="2020-09-25T01:21:42.65" personId="{75DA31A4-1CF0-4DC1-93FC-9A3DBED522DD}" id="{7E5DF10E-9598-4C7A-AC3E-B50A47336E65}">
+    <text>the distance from center of small mass to center of large mass</text>
+  </threadedComment>
+  <threadedComment ref="A82" dT="2020-09-25T01:24:03.30" personId="{75DA31A4-1CF0-4DC1-93FC-9A3DBED522DD}" id="{F95CAA28-D0F2-451C-80BA-B448744334CE}">
+    <text>Mass of the large mass</text>
+  </threadedComment>
+  <threadedComment ref="A83" dT="2020-09-25T01:25:04.35" personId="{75DA31A4-1CF0-4DC1-93FC-9A3DBED522DD}" id="{6B1F4904-C3C9-4912-A741-561A88464FCA}">
+    <text>Distance from meter stick to mirror</text>
+  </threadedComment>
+  <threadedComment ref="A84" dT="2020-09-25T01:26:51.03" personId="{75DA31A4-1CF0-4DC1-93FC-9A3DBED522DD}" id="{A7C83F0A-E0DF-4064-83F0-843BD08DF3F2}">
+    <text>distance of the laser oscillation</text>
+  </threadedComment>
+  <threadedComment ref="A85" dT="2020-09-25T01:27:32.74" personId="{75DA31A4-1CF0-4DC1-93FC-9A3DBED522DD}" id="{27911C3A-1FDB-49D8-8DE3-EDBAEDC01BFB}">
+    <text>Period of oscillation</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7632FA61-5936-4D9A-87FC-59CC7605A5F5}">
-  <dimension ref="A1:H87"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7632FA61-5936-4D9A-87FC-59CC7605A5F5}">
+  <dimension ref="A1:H97"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C87" sqref="C87"/>
+    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="C96" sqref="C96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.6640625" customWidth="1"/>
+    <col min="1" max="1" width="16.33203125" customWidth="1"/>
     <col min="2" max="2" width="16" customWidth="1"/>
     <col min="3" max="3" width="14.77734375" customWidth="1"/>
     <col min="5" max="5" width="18.44140625" customWidth="1"/>
@@ -2161,6 +2325,9 @@
       <c r="F20">
         <v>110</v>
       </c>
+      <c r="G20">
+        <v>5</v>
+      </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" s="2">
@@ -2178,6 +2345,9 @@
       <c r="F21">
         <v>370</v>
       </c>
+      <c r="G21">
+        <v>5</v>
+      </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" s="2">
@@ -2196,6 +2366,10 @@
         <f>F21-F20</f>
         <v>260</v>
       </c>
+      <c r="G22">
+        <f>G20+G21</f>
+        <v>10</v>
+      </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" s="2">
@@ -2214,6 +2388,10 @@
         <f>F22*2</f>
         <v>520</v>
       </c>
+      <c r="G23">
+        <f>G22*2</f>
+        <v>20</v>
+      </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" s="2">
@@ -2517,7 +2695,7 @@
       <c r="A50" s="2">
         <v>310</v>
       </c>
-      <c r="B50">
+      <c r="B50" s="1">
         <v>63</v>
       </c>
       <c r="C50">
@@ -2627,7 +2805,7 @@
       <c r="A60" s="2">
         <v>410</v>
       </c>
-      <c r="B60">
+      <c r="B60" s="1">
         <v>64</v>
       </c>
       <c r="C60">
@@ -2715,7 +2893,7 @@
       <c r="A68" s="2">
         <v>490</v>
       </c>
-      <c r="B68">
+      <c r="B68" s="1">
         <v>56</v>
       </c>
       <c r="C68">
@@ -2789,30 +2967,39 @@
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B79">
         <f>9.55/1000</f>
         <v>9.5500000000000012E-3</v>
       </c>
+      <c r="C79">
+        <v>1.0000000000000001E-5</v>
+      </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B80">
         <f>50/1000</f>
         <v>0.05</v>
       </c>
+      <c r="C80">
+        <v>0.01</v>
+      </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B81">
         <f>42.2/1000</f>
         <v>4.2200000000000001E-2</v>
       </c>
+      <c r="C81">
+        <v>2E-3</v>
+      </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
@@ -2821,6 +3008,9 @@
       <c r="B82">
         <v>1.5</v>
       </c>
+      <c r="C82">
+        <v>0.05</v>
+      </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
@@ -2837,7 +3027,7 @@
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B84" s="5">
         <f>G7/100</f>
@@ -2856,14 +3046,80 @@
         <f>F23</f>
         <v>520</v>
       </c>
+      <c r="C85">
+        <f>G23</f>
+        <v>20</v>
+      </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="B87">
         <f>PI()^2*B84*B81^2*((B80^2+(0.4*B79^2))/(B85^2*B82*B83*B80))</f>
         <v>5.6010641366702152E-11</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A88" t="s">
+        <v>29</v>
+      </c>
+      <c r="B88" s="8">
+        <v>6.67E-11</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A89" t="s">
+        <v>30</v>
+      </c>
+      <c r="B89" s="9">
+        <f>ABS(B87-B88)/AVERAGE(B87:B88)</f>
+        <v>0.17422056496884111</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A92" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C93" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A94" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="B94">
+        <f>B81^3/((B81^2+4*B80^2)^(3/2))</f>
+        <v>5.8772337831158858E-2</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="A95" t="s">
+        <v>33</v>
+      </c>
+      <c r="B95">
+        <f>B87/(1-B94)</f>
+        <v>5.9508069745462651E-11</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A96" t="s">
+        <v>29</v>
+      </c>
+      <c r="B96" s="8">
+        <v>6.67E-11</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A97" t="s">
+        <v>30</v>
+      </c>
+      <c r="B97" s="9">
+        <f>ABS(B95-B96)/AVERAGE(B95:B96)</f>
+        <v>0.11396942000685195</v>
       </c>
     </row>
   </sheetData>
@@ -2873,5 +3129,6 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
   <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Calcualte uncertainty of G
</commit_message>
<xml_diff>
--- a/CavendishExperiment.xlsx
+++ b/CavendishExperiment.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JARAINES\Documents\Daniel Litt\CavendishExperiment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{347C3705-3DC9-47F7-B6EB-4D4807043149}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1352187-D30E-42B1-94D5-E8C7EE570E89}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{1D886BEF-429E-4660-9EA4-F3E5EA03BF59}"/>
   </bookViews>
@@ -105,7 +105,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="40">
   <si>
     <t>Measurements of S</t>
   </si>
@@ -221,16 +221,35 @@
   <si>
     <t>Corrected value of G</t>
   </si>
+  <si>
+    <t>equation</t>
+  </si>
+  <si>
+    <t>partial dirivative</t>
+  </si>
+  <si>
+    <t>Uncertainty^2</t>
+  </si>
+  <si>
+    <t>partial dirivative^2</t>
+  </si>
+  <si>
+    <t>Uncertainty^2*partial dirivative^2</t>
+  </si>
+  <si>
+    <t>Uncertainty of G^2</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
+    <numFmt numFmtId="171" formatCode="0.00000"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -273,6 +292,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -311,12 +338,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1"/>
@@ -329,8 +357,11 @@
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="3"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Output" xfId="1" builtinId="21"/>
     <cellStyle name="Percent" xfId="2" builtinId="5"/>
@@ -2042,8 +2073,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7632FA61-5936-4D9A-87FC-59CC7605A5F5}">
   <dimension ref="A1:H97"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="C88" sqref="C88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2051,9 +2082,10 @@
     <col min="1" max="1" width="16.33203125" customWidth="1"/>
     <col min="2" max="2" width="16" customWidth="1"/>
     <col min="3" max="3" width="14.77734375" customWidth="1"/>
+    <col min="4" max="4" width="13" customWidth="1"/>
     <col min="5" max="5" width="18.44140625" customWidth="1"/>
-    <col min="6" max="6" width="13.5546875" customWidth="1"/>
-    <col min="7" max="7" width="13.21875" customWidth="1"/>
+    <col min="6" max="6" width="16.33203125" customWidth="1"/>
+    <col min="7" max="7" width="17" customWidth="1"/>
     <col min="8" max="8" width="14.21875" customWidth="1"/>
     <col min="9" max="9" width="14.6640625" bestFit="1" customWidth="1"/>
   </cols>
@@ -2837,7 +2869,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>460</v>
       </c>
@@ -2848,7 +2880,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>470</v>
       </c>
@@ -2859,7 +2891,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>480</v>
       </c>
@@ -2870,7 +2902,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>490</v>
       </c>
@@ -2881,7 +2913,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>500</v>
       </c>
@@ -2892,7 +2924,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>510</v>
       </c>
@@ -2903,7 +2935,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>520</v>
       </c>
@@ -2914,7 +2946,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A72">
         <v>530</v>
       </c>
@@ -2925,7 +2957,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A73">
         <v>540</v>
       </c>
@@ -2936,17 +2968,29 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C78" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D78" t="s">
+        <v>36</v>
+      </c>
+      <c r="E78" t="s">
+        <v>35</v>
+      </c>
+      <c r="F78" t="s">
+        <v>37</v>
+      </c>
+      <c r="G78" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>24</v>
       </c>
@@ -2957,8 +3001,27 @@
       <c r="C79">
         <v>1.0000000000000001E-5</v>
       </c>
-    </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D79">
+        <f>C79^2</f>
+        <v>1.0000000000000002E-10</v>
+      </c>
+      <c r="E79">
+        <f>(4*PI()^2*B81^2*B84*B79)/(5*B80*B83*B85^2*B82)</f>
+        <v>1.6870668459239571E-10</v>
+      </c>
+      <c r="F79">
+        <f>E79^2</f>
+        <v>2.8461945426158088E-20</v>
+      </c>
+      <c r="G79">
+        <f>D79*F79</f>
+        <v>2.8461945426158092E-30</v>
+      </c>
+      <c r="H79" s="11" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>25</v>
       </c>
@@ -2969,8 +3032,27 @@
       <c r="C80">
         <v>0.01</v>
       </c>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D80">
+        <f t="shared" ref="D80:D85" si="1">C80^2</f>
+        <v>1E-4</v>
+      </c>
+      <c r="E80">
+        <f>(PI()^2*$B$81^2*$B$84*(5*$B$80^2-2*$B$79^2))/(5*$B$80^2*$B$83*$B$85^2*$B$82)</f>
+        <v>1.0879898505768954E-9</v>
+      </c>
+      <c r="F80">
+        <f t="shared" ref="F80:F85" si="2">E80^2</f>
+        <v>1.1837219149583353E-18</v>
+      </c>
+      <c r="G80">
+        <f t="shared" ref="G80:G85" si="3">D80*F80</f>
+        <v>1.1837219149583355E-22</v>
+      </c>
+      <c r="H80" s="11" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>26</v>
       </c>
@@ -2981,8 +3063,27 @@
       <c r="C81">
         <v>2E-3</v>
       </c>
-    </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D81">
+        <f t="shared" si="1"/>
+        <v>3.9999999999999998E-6</v>
+      </c>
+      <c r="E81">
+        <f>(2*PI()^2*$B$81*$B$84*(5*$B$80^2+2*$B$79^2))/(5*$B$80*$B$83*$B$85^2*$B$82)</f>
+        <v>2.654532766194415E-9</v>
+      </c>
+      <c r="F81">
+        <f t="shared" si="2"/>
+        <v>7.0465442067997726E-18</v>
+      </c>
+      <c r="G81">
+        <f t="shared" si="3"/>
+        <v>2.818617682719909E-23</v>
+      </c>
+      <c r="H81" s="11" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="82" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>22</v>
       </c>
@@ -2992,8 +3093,27 @@
       <c r="C82">
         <v>0.05</v>
       </c>
-    </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D82">
+        <f t="shared" si="1"/>
+        <v>2.5000000000000005E-3</v>
+      </c>
+      <c r="E82">
+        <f>-(PI()^2*$B$81^2*$B$84*(5*$B$80^2+2*$B$79^2))/(5*$B$80*$B$83*$B$85^2*$B$82^2)</f>
+        <v>-3.7340427577801437E-11</v>
+      </c>
+      <c r="F82">
+        <f t="shared" si="2"/>
+        <v>1.3943075316930341E-21</v>
+      </c>
+      <c r="G82">
+        <f t="shared" si="3"/>
+        <v>3.4857688292325855E-24</v>
+      </c>
+      <c r="H82" s="11" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="83" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>19</v>
       </c>
@@ -3005,8 +3125,27 @@
         <f>G26</f>
         <v>0.02</v>
       </c>
-    </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D83">
+        <f t="shared" si="1"/>
+        <v>4.0000000000000002E-4</v>
+      </c>
+      <c r="E83">
+        <f>-(PI()^2*$B$81^2*$B$84*(5*$B$80^2+2*$B$79^2))/(5*$B$80*$B$83^2*$B$85^2*$B$82)</f>
+        <v>-9.4135531708743121E-12</v>
+      </c>
+      <c r="F83">
+        <f t="shared" si="2"/>
+        <v>8.8614983300877817E-23</v>
+      </c>
+      <c r="G83">
+        <f t="shared" si="3"/>
+        <v>3.5445993320351131E-26</v>
+      </c>
+      <c r="H83" s="11" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="84" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>27</v>
       </c>
@@ -3018,8 +3157,27 @@
         <f>H7/100</f>
         <v>3.5377331097124383E-3</v>
       </c>
-    </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D84">
+        <f t="shared" si="1"/>
+        <v>1.2515555555555638E-5</v>
+      </c>
+      <c r="E84">
+        <f>(PI()^2*$B$81^2*(5*$B$80^2+2*$B$79^2))/(5*$B$80*$B$83*$B$85^2*$B$82)</f>
+        <v>3.6946333355344443E-10</v>
+      </c>
+      <c r="F84">
+        <f t="shared" si="2"/>
+        <v>1.3650315484042375E-19</v>
+      </c>
+      <c r="G84">
+        <f t="shared" si="3"/>
+        <v>1.708412817913937E-24</v>
+      </c>
+      <c r="H84" s="11" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="85" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>13</v>
       </c>
@@ -3031,8 +3189,36 @@
         <f>G23</f>
         <v>20</v>
       </c>
-    </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D85">
+        <f t="shared" si="1"/>
+        <v>400</v>
+      </c>
+      <c r="E85">
+        <f>-(2*PI()^2*$B$81^2*$B$84*(5*$B$80^2+2*$B$79^2))/(5*$B$80*$B$83*$B$85^3*$B$82)</f>
+        <v>-2.1542554371808521E-13</v>
+      </c>
+      <c r="F85">
+        <f t="shared" si="2"/>
+        <v>4.640816488623264E-26</v>
+      </c>
+      <c r="G85">
+        <f t="shared" si="3"/>
+        <v>1.8563265954493056E-23</v>
+      </c>
+      <c r="H85" s="11" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="86" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="F86" t="s">
+        <v>39</v>
+      </c>
+      <c r="G86">
+        <f>SUM(G79:G85)</f>
+        <v>1.7035126476418712E-22</v>
+      </c>
+    </row>
+    <row r="87" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>28</v>
       </c>
@@ -3040,8 +3226,12 @@
         <f>PI()^2*B84*B81^2*((B80^2+(0.4*B79^2))/(B85^2*B82*B83*B80))</f>
         <v>5.6010641366702152E-11</v>
       </c>
-    </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C87">
+        <f>SQRT(G86)</f>
+        <v>1.3051868248039708E-11</v>
+      </c>
+    </row>
+    <row r="88" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>29</v>
       </c>
@@ -3049,7 +3239,7 @@
         <v>6.67E-11</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>30</v>
       </c>
@@ -3058,26 +3248,26 @@
         <v>0.17422056496884111</v>
       </c>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C93" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A94" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="B94">
+      <c r="B94" s="10">
         <f>B81^3/((B81^2+4*B80^2)^(3/2))</f>
         <v>5.8772337831158858E-2</v>
       </c>
     </row>
-    <row r="95" spans="1:3" ht="15.6" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:8" ht="15.6" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
         <v>32</v>
       </c>
@@ -3086,7 +3276,7 @@
         <v>5.9508069745462651E-11</v>
       </c>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>29</v>
       </c>
@@ -3107,9 +3297,19 @@
   <mergeCells count="1">
     <mergeCell ref="F3:G3"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="H79" r:id="rId1" display="test" xr:uid="{6BEC0A57-AC6C-46F4-ABBB-9B08BA02DDC8}"/>
+    <hyperlink ref="H80" r:id="rId2" xr:uid="{8E3D35C6-E0FE-4CED-8C6D-C4FB833FD958}"/>
+    <hyperlink ref="H81" r:id="rId3" xr:uid="{4F2BE297-9C19-4C3F-AC29-73635DE7610D}"/>
+    <hyperlink ref="H82:H85" r:id="rId4" display="equation" xr:uid="{471637F7-9FCC-4596-9A91-5882FB08C20D}"/>
+    <hyperlink ref="H82" r:id="rId5" xr:uid="{0787D4CC-4A8F-489F-8462-B3108CCE7D5C}"/>
+    <hyperlink ref="H83" r:id="rId6" xr:uid="{4150FE10-8621-4CD1-A419-15D47FF5CE98}"/>
+    <hyperlink ref="H84" r:id="rId7" xr:uid="{AAAC84C2-A602-49DE-969A-35007672298A}"/>
+    <hyperlink ref="H85" r:id="rId8" xr:uid="{9BC23F37-3331-407F-BC5E-A26B831A40C1}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
-  <drawing r:id="rId2"/>
-  <legacyDrawing r:id="rId3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId9"/>
+  <drawing r:id="rId10"/>
+  <legacyDrawing r:id="rId11"/>
 </worksheet>
 </file>
</xml_diff>